<commit_message>
Updated LED current usage details.
</commit_message>
<xml_diff>
--- a/LED mAmps.xlsx
+++ b/LED mAmps.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\YABEIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795BA385-750C-4AC2-973B-A7A87FED096A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74A99BC-665B-4399-88E5-0014ABA1DAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8539FAA7-9EEC-4735-872C-E57BBCD9C901}"/>
   </bookViews>
@@ -270,19 +270,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>5.9</c:v>
+                  <c:v>5.7550000000000008</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.37</c:v>
+                  <c:v>17.913999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26</c:v>
+                  <c:v>25.72</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35</c:v>
+                  <c:v>34.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44.1</c:v>
+                  <c:v>43.85</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>53.7</c:v>
@@ -1422,9 +1422,12 @@
       <c r="B2">
         <v>5.9</v>
       </c>
+      <c r="C2">
+        <v>5.61</v>
+      </c>
       <c r="H2">
         <f t="shared" ref="H2:H14" si="0">AVERAGE(B2:F2)</f>
-        <v>5.9</v>
+        <v>5.7550000000000008</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1434,9 +1437,21 @@
       <c r="B3">
         <v>16.37</v>
       </c>
+      <c r="C3">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="D3">
+        <v>15.7</v>
+      </c>
+      <c r="E3">
+        <v>25.1</v>
+      </c>
+      <c r="F3">
+        <v>16</v>
+      </c>
       <c r="H3">
         <f t="shared" si="0"/>
-        <v>16.37</v>
+        <v>17.913999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1446,9 +1461,21 @@
       <c r="B4">
         <v>26</v>
       </c>
+      <c r="C4">
+        <v>25.8</v>
+      </c>
+      <c r="D4">
+        <v>25.8</v>
+      </c>
+      <c r="E4">
+        <v>26</v>
+      </c>
+      <c r="F4">
+        <v>25</v>
+      </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>25.72</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1458,9 +1485,21 @@
       <c r="B5">
         <v>35</v>
       </c>
+      <c r="C5">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="D5">
+        <v>34.9</v>
+      </c>
+      <c r="E5">
+        <v>35.1</v>
+      </c>
+      <c r="F5">
+        <v>34.299999999999997</v>
+      </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>34.799999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1470,9 +1509,12 @@
       <c r="B6">
         <v>44.1</v>
       </c>
+      <c r="C6">
+        <v>43.6</v>
+      </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>44.1</v>
+        <v>43.85</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>